<commit_message>
upd averages excels+plot code
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_500.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_500.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,17 +471,42 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Experiment_Time</t>
+          <t>Avg_Experiment_Time</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Std_Total_Rounds</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Std_Expl_Cost</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Std_Expl_Eff</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Std_Round_Time</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Std_Agent_Step_Time</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Std_Experiment_Time</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Obs_Prob</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Std_Total_Rounds</t>
         </is>
       </c>
     </row>
@@ -493,28 +518,43 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>86.63</v>
+        <v>53.68</v>
       </c>
       <c r="D2" t="n">
-        <v>86.63</v>
+        <v>53.68</v>
       </c>
       <c r="E2" t="n">
-        <v>1.98704</v>
+        <v>3.17812994</v>
       </c>
       <c r="F2" t="n">
-        <v>0.11754</v>
+        <v>0.16001446</v>
       </c>
       <c r="G2" t="n">
-        <v>0.11754</v>
+        <v>0.16001446</v>
       </c>
       <c r="H2" t="n">
-        <v>10.0728</v>
+        <v>8.5570018</v>
       </c>
       <c r="I2" t="n">
-        <v>0.85</v>
+        <v>5.147678816164503</v>
       </c>
       <c r="J2" t="n">
-        <v>11.94458</v>
+        <v>5.147678816164503</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.3145584481778171</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.01588193493321408</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.01588193493321408</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.9109293698347942</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="3">
@@ -525,28 +565,43 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>53.68</v>
+        <v>86.63</v>
       </c>
       <c r="D3" t="n">
-        <v>53.68</v>
+        <v>86.63</v>
       </c>
       <c r="E3" t="n">
-        <v>3.17813</v>
+        <v>1.98703528</v>
       </c>
       <c r="F3" t="n">
-        <v>0.16001</v>
+        <v>0.11753604</v>
       </c>
       <c r="G3" t="n">
-        <v>0.16001</v>
+        <v>0.11753604</v>
       </c>
       <c r="H3" t="n">
-        <v>8.557</v>
+        <v>10.07280072</v>
       </c>
       <c r="I3" t="n">
-        <v>0.15</v>
+        <v>11.95654707831956</v>
       </c>
       <c r="J3" t="n">
-        <v>5.14253</v>
+        <v>11.95654707831956</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.268514152512527</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.02131027097002833</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.02131027097002833</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.760146952548398</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="4">
@@ -563,22 +618,37 @@
         <v>61.97</v>
       </c>
       <c r="E4" t="n">
-        <v>2.78323</v>
+        <v>2.78322638</v>
       </c>
       <c r="F4" t="n">
-        <v>0.28506</v>
+        <v>0.2850598</v>
       </c>
       <c r="G4" t="n">
-        <v>0.14253</v>
+        <v>0.14252968</v>
       </c>
       <c r="H4" t="n">
-        <v>4.39695</v>
+        <v>4.396953860000001</v>
       </c>
       <c r="I4" t="n">
+        <v>4.475717606841654</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8.919204247510965</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.3964916854618472</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.04660330493453917</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0233015466708136</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.8670662738777775</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.15</v>
-      </c>
-      <c r="J4" t="n">
-        <v>4.47124</v>
       </c>
     </row>
     <row r="5">
@@ -595,22 +665,37 @@
         <v>93.294</v>
       </c>
       <c r="E5" t="n">
-        <v>1.85185</v>
+        <v>1.85185002</v>
       </c>
       <c r="F5" t="n">
-        <v>0.18284</v>
+        <v>0.18283646</v>
       </c>
       <c r="G5" t="n">
-        <v>0.09142</v>
+        <v>0.09141832</v>
       </c>
       <c r="H5" t="n">
-        <v>4.28448</v>
+        <v>4.28448244</v>
       </c>
       <c r="I5" t="n">
+        <v>7.765951068091015</v>
+      </c>
+      <c r="J5" t="n">
+        <v>14.16137893379784</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.2725678101817861</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.03187944356968964</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.01593986758837946</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.7113420070683908</v>
+      </c>
+      <c r="O5" t="n">
         <v>0.85</v>
-      </c>
-      <c r="J5" t="n">
-        <v>7.75818</v>
       </c>
     </row>
     <row r="6">
@@ -621,28 +706,43 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>26.634</v>
+        <v>18.638</v>
       </c>
       <c r="D6" t="n">
-        <v>98.578</v>
+        <v>74.416</v>
       </c>
       <c r="E6" t="n">
-        <v>1.74627</v>
+        <v>2.32578502</v>
       </c>
       <c r="F6" t="n">
-        <v>0.27419</v>
+        <v>0.36064252</v>
       </c>
       <c r="G6" t="n">
-        <v>0.06855</v>
+        <v>0.09016050000000002</v>
       </c>
       <c r="H6" t="n">
-        <v>1.8096</v>
+        <v>1.68161806</v>
       </c>
       <c r="I6" t="n">
-        <v>0.85</v>
+        <v>2.923705201317058</v>
       </c>
       <c r="J6" t="n">
-        <v>4.33175</v>
+        <v>11.70114428400531</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.3594154407059264</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.08021947645837707</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.02005467182663801</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.463798327492031</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="7">
@@ -653,28 +753,43 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>18.638</v>
+        <v>26.634</v>
       </c>
       <c r="D7" t="n">
-        <v>74.416</v>
+        <v>98.578</v>
       </c>
       <c r="E7" t="n">
-        <v>2.32579</v>
+        <v>1.74627016</v>
       </c>
       <c r="F7" t="n">
-        <v>0.36064</v>
+        <v>0.27419382</v>
       </c>
       <c r="G7" t="n">
-        <v>0.09016</v>
+        <v>0.06854842</v>
       </c>
       <c r="H7" t="n">
-        <v>1.68162</v>
+        <v>1.80959682</v>
       </c>
       <c r="I7" t="n">
-        <v>0.15</v>
+        <v>4.336086633658186</v>
       </c>
       <c r="J7" t="n">
-        <v>2.92078</v>
+        <v>13.43640539653221</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.2387359758249279</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.06370485136771897</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.01592628321667663</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4464294974852552</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="8">
@@ -691,22 +806,37 @@
         <v>75.88800000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>2.31683</v>
+        <v>2.31683128</v>
       </c>
       <c r="F8" t="n">
-        <v>0.41166</v>
+        <v>0.41165586</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06861</v>
+        <v>0.06860936000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>0.87713</v>
+        <v>0.8771295800000001</v>
       </c>
       <c r="I8" t="n">
+        <v>2.308339850570419</v>
+      </c>
+      <c r="J8" t="n">
+        <v>13.8082871344412</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.5191305164231101</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.1192346384902147</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.01987252630628497</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.3294023284148944</v>
+      </c>
+      <c r="O8" t="n">
         <v>0.15</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2.30603</v>
       </c>
     </row>
     <row r="9">
@@ -723,22 +853,37 @@
         <v>95.774</v>
       </c>
       <c r="E9" t="n">
-        <v>1.80873</v>
+        <v>1.80873238</v>
       </c>
       <c r="F9" t="n">
-        <v>0.28884</v>
+        <v>0.28884228</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04814</v>
+        <v>0.04814038</v>
       </c>
       <c r="H9" t="n">
-        <v>0.89345</v>
+        <v>0.8934506799999999</v>
       </c>
       <c r="I9" t="n">
+        <v>3.704306652472376</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14.76912923488428</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.2942889472751435</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.07352609914658213</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.01225404545918741</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2778735680592697</v>
+      </c>
+      <c r="O9" t="n">
         <v>0.85</v>
-      </c>
-      <c r="J9" t="n">
-        <v>3.7006</v>
       </c>
     </row>
     <row r="10">
@@ -749,28 +894,43 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>14.542</v>
+        <v>9.528</v>
       </c>
       <c r="D10" t="n">
-        <v>90.11</v>
+        <v>76.026</v>
       </c>
       <c r="E10" t="n">
-        <v>1.94035</v>
+        <v>2.34660458</v>
       </c>
       <c r="F10" t="n">
-        <v>0.26271</v>
+        <v>0.36560598</v>
       </c>
       <c r="G10" t="n">
-        <v>0.03284</v>
+        <v>0.04570056</v>
       </c>
       <c r="H10" t="n">
-        <v>0.47596</v>
+        <v>0.44229886</v>
       </c>
       <c r="I10" t="n">
-        <v>0.85</v>
+        <v>2.134086373439135</v>
       </c>
       <c r="J10" t="n">
-        <v>3.72937</v>
+        <v>17.03248470042291</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.5813009885408598</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.1120422344700859</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.01400517053411987</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1910490882520623</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="11">
@@ -781,28 +941,43 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>9.528</v>
+        <v>14.542</v>
       </c>
       <c r="D11" t="n">
-        <v>76.026</v>
+        <v>90.11</v>
       </c>
       <c r="E11" t="n">
-        <v>2.34661</v>
+        <v>1.94034866</v>
       </c>
       <c r="F11" t="n">
-        <v>0.36561</v>
+        <v>0.26271068</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0457</v>
+        <v>0.03283892</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4423</v>
+        <v>0.4759576599999999</v>
       </c>
       <c r="I11" t="n">
-        <v>0.15</v>
+        <v>3.733109724670957</v>
       </c>
       <c r="J11" t="n">
-        <v>2.13195</v>
+        <v>16.53410576071815</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.3659283612363473</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.07516614324360295</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.009395605954706286</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.1918604916329145</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="12">
@@ -819,22 +994,37 @@
         <v>72.416</v>
       </c>
       <c r="E12" t="n">
-        <v>2.49797</v>
+        <v>2.49796812</v>
       </c>
       <c r="F12" t="n">
-        <v>0.35798</v>
+        <v>0.35798356</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0358</v>
+        <v>0.0357984</v>
       </c>
       <c r="H12" t="n">
-        <v>0.26875</v>
+        <v>0.26875334</v>
       </c>
       <c r="I12" t="n">
+        <v>1.828932472229621</v>
+      </c>
+      <c r="J12" t="n">
+        <v>18.25248614575565</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.6916429980740318</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.1215264625450928</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.01215267791892809</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.1392939107174838</v>
+      </c>
+      <c r="O12" t="n">
         <v>0.15</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1.8271</v>
       </c>
     </row>
     <row r="13">
@@ -851,22 +1041,37 @@
         <v>84.27200000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>2.08263</v>
+        <v>2.08262574</v>
       </c>
       <c r="F13" t="n">
-        <v>0.23579</v>
+        <v>0.23579416</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02358</v>
+        <v>0.02357946</v>
       </c>
       <c r="H13" t="n">
-        <v>0.28097</v>
+        <v>0.2809738</v>
       </c>
       <c r="I13" t="n">
+        <v>3.304806725814685</v>
+      </c>
+      <c r="J13" t="n">
+        <v>16.52198438250901</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.4083749073524997</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.06549908709527966</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.006549929454591113</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.11199575969267</v>
+      </c>
+      <c r="O13" t="n">
         <v>0.85</v>
-      </c>
-      <c r="J13" t="n">
-        <v>3.3015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recalc avg+code for all_avg excel
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_500.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_500.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>